<commit_message>
Added "temp_library.lbr" to eagle folder. Updated Power requirements excel documentation.
</commit_message>
<xml_diff>
--- a/Documentation/Power Requirements - Controller Board.xlsx
+++ b/Documentation/Power Requirements - Controller Board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19155" windowHeight="8505"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19155" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Power Supplies" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Device</t>
   </si>
@@ -26,15 +26,6 @@
     <t>AD8616R-8</t>
   </si>
   <si>
-    <t>TPD4S012</t>
-  </si>
-  <si>
-    <t>TLK110</t>
-  </si>
-  <si>
-    <t>LTC4263</t>
-  </si>
-  <si>
     <t>ADC</t>
   </si>
   <si>
@@ -45,9 +36,6 @@
   </si>
   <si>
     <t>PoE REGULATOR</t>
-  </si>
-  <si>
-    <t>USB PROTECTOR</t>
   </si>
   <si>
     <t>Required Voltage (V)</t>
@@ -133,6 +121,16 @@
   </si>
   <si>
     <t>Analog Reference Voltage Regulator (8.0V)</t>
+  </si>
+  <si>
+    <t>KSZ8081</t>
+  </si>
+  <si>
+    <t>MAX5984C</t>
+  </si>
+  <si>
+    <t>Required 
+Current (mA)</t>
   </si>
 </sst>
 </file>
@@ -174,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -414,11 +412,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -531,6 +592,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -829,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -845,23 +927,23 @@
     <row r="1" spans="2:12" ht="10.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:12">
       <c r="B2" s="38" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C2" s="40" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="37"/>
       <c r="G2" s="35" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H2" s="36"/>
       <c r="I2" s="37"/>
       <c r="J2" s="35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K2" s="36"/>
       <c r="L2" s="37"/>
@@ -870,45 +952,45 @@
       <c r="B3" s="39"/>
       <c r="C3" s="41"/>
       <c r="D3" s="23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="20">
         <v>4.5</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" s="22">
         <v>42</v>
@@ -926,7 +1008,7 @@
         <v>350</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L4" s="22">
         <v>900</v>
@@ -934,16 +1016,16 @@
     </row>
     <row r="5" spans="2:12">
       <c r="B5" s="18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="20">
         <v>5.7</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F5" s="22">
         <v>42</v>
@@ -961,7 +1043,7 @@
         <v>430</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L5" s="22">
         <v>900</v>
@@ -969,16 +1051,16 @@
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="6">
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F6" s="7">
         <v>18</v>
@@ -996,7 +1078,7 @@
         <v>-20</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L6" s="7">
         <v>30</v>
@@ -1004,10 +1086,10 @@
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D7" s="6">
         <v>9</v>
@@ -1039,16 +1121,16 @@
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6">
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F8" s="7">
         <v>42</v>
@@ -1057,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I8" s="7">
         <v>30</v>
@@ -1074,16 +1156,16 @@
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1">
       <c r="B9" s="13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9" s="8">
         <v>9</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F9" s="10">
         <v>36</v>
@@ -1097,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L9" s="10">
         <v>1560</v>
@@ -1118,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H15"/>
+  <dimension ref="B1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1130,49 +1212,54 @@
     <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
     <col min="4" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="14.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="12.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:8" s="4" customFormat="1">
+    <row r="1" spans="2:9" ht="12.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:9" s="4" customFormat="1">
       <c r="B2" s="38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="40" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="37"/>
-      <c r="G2" s="42" t="s">
-        <v>15</v>
+      <c r="G2" s="50" t="s">
+        <v>37</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="15.75" thickBot="1">
+        <v>11</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="B3" s="39"/>
       <c r="C3" s="41"/>
       <c r="D3" s="23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="43"/>
+        <v>10</v>
+      </c>
+      <c r="G3" s="49"/>
       <c r="H3" s="43"/>
-    </row>
-    <row r="4" spans="2:8">
+      <c r="I3" s="43"/>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" s="18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>1</v>
@@ -1186,16 +1273,19 @@
       <c r="F4" s="22">
         <v>5.5</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="45">
+        <v>3</v>
+      </c>
+      <c r="H4" s="26">
         <v>15</v>
       </c>
-      <c r="H4" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="I4" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" s="11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>1</v>
@@ -1209,16 +1299,19 @@
       <c r="F5" s="7">
         <v>5.5</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="46">
+        <v>3</v>
+      </c>
+      <c r="H5" s="15">
         <v>15</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
+      <c r="I5" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6" s="11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>1</v>
@@ -1232,16 +1325,19 @@
       <c r="F6" s="7">
         <v>5.5</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="46">
+        <v>3</v>
+      </c>
+      <c r="H6" s="15">
         <v>15</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8">
+      <c r="I6" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" s="11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>1</v>
@@ -1255,16 +1351,19 @@
       <c r="F7" s="7">
         <v>5.5</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="46">
+        <v>3</v>
+      </c>
+      <c r="H7" s="15">
         <v>15</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8">
+      <c r="I7" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" s="11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>2</v>
@@ -1276,14 +1375,17 @@
       <c r="F8" s="7">
         <v>5.5</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
+      <c r="G8" s="46">
+        <v>150</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" s="11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>2</v>
@@ -1295,14 +1397,17 @@
       <c r="F9" s="7">
         <v>5.5</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8">
+      <c r="G9" s="46">
+        <v>150</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" s="11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>2</v>
@@ -1314,14 +1419,17 @@
       <c r="F10" s="7">
         <v>5.5</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="G10" s="46">
+        <v>150</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
       <c r="B11" s="11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>2</v>
@@ -1333,108 +1441,100 @@
       <c r="F11" s="7">
         <v>5.5</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="46">
+        <v>150</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="D12" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="G12" s="46">
+        <v>152</v>
+      </c>
+      <c r="H12" s="15">
+        <v>500</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13" s="11" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1.8</v>
+        <v>35</v>
+      </c>
+      <c r="D13" s="32">
+        <v>3.1349999999999998</v>
       </c>
       <c r="E13" s="5">
         <v>3.3</v>
       </c>
-      <c r="F13" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="G13" s="15">
-        <v>500</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6">
-        <v>3</v>
-      </c>
-      <c r="E14" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="F14" s="7">
-        <v>3.6</v>
-      </c>
-      <c r="G14" s="16">
-        <v>200</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B15" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="8">
-        <v>46</v>
-      </c>
-      <c r="E15" s="9">
-        <v>48</v>
-      </c>
-      <c r="F15" s="10">
-        <v>57</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17" t="s">
-        <v>25</v>
+      <c r="F13" s="34">
+        <v>3.46</v>
+      </c>
+      <c r="G13" s="47">
+        <v>47</v>
+      </c>
+      <c r="H13" s="16">
+        <v>155</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="8">
+        <v>32</v>
+      </c>
+      <c r="E14" s="9">
+        <v>54</v>
+      </c>
+      <c r="F14" s="10">
+        <v>60</v>
+      </c>
+      <c r="G14" s="48">
+        <v>740</v>
+      </c>
+      <c r="H14" s="44">
+        <v>40000</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="G2:G3"/>
+  <mergeCells count="6">
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>